<commit_message>
add fivering list site-category
</commit_message>
<xml_diff>
--- a/duyi/25期基础预备班学习计划宣言表(3).xlsx
+++ b/duyi/25期基础预备班学习计划宣言表(3).xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20377"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\frontend-demo-practices\duyi\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBD4650-383B-4AA9-8F03-F0D603344D83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="9420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,10 +139,6 @@
     <t>【录播】css企业开发经验、习惯，盒子模型，层模型</t>
   </si>
   <si>
-    <t xml:space="preserve">
-【录播】居中五环，两栏布局，两个经典bug，BFC</t>
-  </si>
-  <si>
     <t>【录播】文字溢出处理，背景图片处理，企业开发经验
 【录播】css 升华篇 - css要点补充说明</t>
   </si>
@@ -352,12 +354,17 @@
     <t>【直播】js第八课《笔面试题知识点讲解》</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve">
+【录播】居中五环，两栏布局，两个经典bug，BFC</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -572,10 +579,18 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1"/>
+    <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -865,23 +880,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="24.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57.1796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="24.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="57.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="56.5" customHeight="1">
+    <row r="1" spans="1:7" ht="56.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -896,7 +911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1">
+    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>44427</v>
       </c>
@@ -907,13 +922,13 @@
         <v>5</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" customHeight="1">
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>44428</v>
       </c>
@@ -921,16 +936,16 @@
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" customHeight="1">
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>44429</v>
       </c>
@@ -938,10 +953,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>44430</v>
       </c>
@@ -949,16 +964,16 @@
         <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" customHeight="1">
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>44431</v>
       </c>
@@ -966,301 +981,301 @@
         <v>10</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>44432</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
+      <c r="B7" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" customHeight="1">
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>44433</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>44434</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="9"/>
       <c r="G9" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1">
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="14">
         <v>44435</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" customHeight="1">
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="14">
         <v>44436</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14">
         <v>44437</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" customHeight="1">
+    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="14">
         <v>44438</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="14">
         <v>44439</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
+    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="14">
         <v>44440</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" customHeight="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="14">
         <v>44441</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" customHeight="1">
+    <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="14">
         <v>44442</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:5" ht="30" customHeight="1">
+    <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="14">
         <v>44443</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" customHeight="1">
+    <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="14">
         <v>44444</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1">
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="14">
         <v>44445</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" customHeight="1">
+    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="14">
         <v>44446</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
     </row>
-    <row r="24" spans="1:5" ht="30" customHeight="1">
+    <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="14">
         <v>44447</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" customHeight="1">
+    <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="14">
         <v>44448</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="1:5" ht="30" customHeight="1">
+    <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="14">
         <v>44449</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" customHeight="1">
+    <row r="27" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="14">
         <v>44450</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="E27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" customHeight="1">
+    <row r="28" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" customHeight="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" customHeight="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="8"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:31" ht="37.5" customHeight="1">
+    <row r="33" spans="1:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -1293,9 +1308,9 @@
       <c r="AD33" s="15"/>
       <c r="AE33" s="15"/>
     </row>
-    <row r="34" spans="1:31" ht="100.5" customHeight="1">
+    <row r="34" spans="1:31" ht="100.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -1328,9 +1343,9 @@
       <c r="AD34" s="15"/>
       <c r="AE34" s="15"/>
     </row>
-    <row r="35" spans="1:31" ht="83" customHeight="1">
+    <row r="35" spans="1:31" ht="83.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" s="16"/>
       <c r="C35" s="17"/>
@@ -1363,19 +1378,19 @@
       <c r="AD35" s="17"/>
       <c r="AE35" s="18"/>
     </row>
-    <row r="37" spans="1:31" ht="25.5">
+    <row r="37" spans="1:31" ht="25.5" x14ac:dyDescent="0.15">
       <c r="C37" s="10"/>
     </row>
-    <row r="38" spans="1:31" ht="25.5">
+    <row r="38" spans="1:31" ht="25.5" x14ac:dyDescent="0.15">
       <c r="C38" s="10"/>
     </row>
-    <row r="42" spans="1:31" ht="29.5" customHeight="1">
+    <row r="42" spans="1:31" ht="29.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C42" s="8"/>
     </row>
-    <row r="43" spans="1:31" ht="67" customHeight="1">
+    <row r="43" spans="1:31" ht="66.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C43" s="11"/>
     </row>
-    <row r="45" spans="1:31" ht="31" customHeight="1">
+    <row r="45" spans="1:31" ht="30.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C45" s="8"/>
     </row>
   </sheetData>
@@ -1391,12 +1406,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1404,12 +1419,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>